<commit_message>
v2 change heatsink,reduce shell to 1.5mm, dm base, remove base hole without out 2d draw
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\yj\microscope_design\LaserBox\micolaser_1400\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\yj\microscope_design\LaserBox\micolaser_1400_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA122E64-81FB-4311-AC6A-8EA593B8E66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF7D8B-095F-45CA-84C4-A8C66BCE2A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DFEBBC-1571-4440-9336-F0CA4138F7AF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{10DFEBBC-1571-4440-9336-F0CA4138F7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
+    <t>catalog</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -483,12 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
@@ -500,6 +494,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -819,7 +819,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -871,7 +871,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -896,7 +896,7 @@
         <f>G2*H2</f>
         <v>14500</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -904,7 +904,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="9"/>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="9"/>
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -955,7 +955,7 @@
         <f t="shared" si="0"/>
         <v>37500</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -963,7 +963,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -1016,7 +1016,7 @@
         <f t="shared" si="0"/>
         <v>467.29</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="9"/>
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1044,7 +1044,7 @@
         <f t="shared" si="0"/>
         <v>1145.6400000000001</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1052,7 +1052,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1071,7 +1071,7 @@
         <f t="shared" si="0"/>
         <v>1594.96</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="9"/>
       <c r="D9" s="1" t="s">
         <v>64</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="9"/>
       <c r="D10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C11" t="s">
@@ -1159,7 +1159,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="9"/>
       <c r="C12" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1187,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1206,7 +1206,7 @@
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="9"/>
       <c r="D14" s="1" t="s">
         <v>82</v>
       </c>
@@ -1231,7 +1231,7 @@
         <f t="shared" si="0"/>
         <v>4800</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1239,7 +1239,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="9"/>
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1256,7 +1256,7 @@
         <f t="shared" si="0"/>
         <v>5440</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
@@ -1313,20 +1313,20 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="9"/>
       <c r="C18" t="s">
         <v>35</v>
       </c>
@@ -1346,18 +1346,18 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1387,7 +1387,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
         <v>39</v>
@@ -1413,7 +1413,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="2"/>
@@ -1441,7 +1441,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
         <v>43</v>
@@ -1467,7 +1467,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
         <v>44</v>
@@ -1493,7 +1493,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
         <v>45</v>
@@ -1519,7 +1519,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="2"/>
@@ -1547,7 +1547,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>47</v>
@@ -1573,7 +1573,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>48</v>
@@ -1599,7 +1599,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3" t="s">
         <v>49</v>
@@ -1625,29 +1625,29 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="6" t="s">
         <v>88</v>
       </c>
       <c r="F29" t="s">
         <v>90</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>16</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="7">
         <v>6.84</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="7">
         <f t="shared" si="0"/>
         <v>109.44</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1655,17 +1655,17 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="9"/>
       <c r="D30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>8</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="7">
         <v>7</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="7">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
@@ -1678,13 +1678,13 @@
       <c r="D31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>4</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="7">
         <v>7</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -1705,7 +1705,7 @@
       <c r="G32">
         <v>17</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="7">
         <v>1</v>
       </c>
       <c r="I32">
@@ -1726,7 +1726,7 @@
       <c r="G33">
         <v>28</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="7">
         <v>1</v>
       </c>
       <c r="I33">
@@ -1747,7 +1747,7 @@
       <c r="G34">
         <v>16</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="7">
         <v>0.5</v>
       </c>
       <c r="I34">
@@ -1769,16 +1769,16 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="J17:O18"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B11:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
mifigy shell ans base for manufaction
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\yj\microscope_design\LaserBox\micolaser_1400_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF7D8B-095F-45CA-84C4-A8C66BCE2A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8249880B-FBA2-49F2-9478-C6956FBA50DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{10DFEBBC-1571-4440-9336-F0CA4138F7AF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DFEBBC-1571-4440-9336-F0CA4138F7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -404,6 +404,12 @@
   <si>
     <t>catalog</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定位销 圆柱型/A型/m6正公差_价格_多少钱_图片-米思米官网 (misumi.com.cn)</t>
+  </si>
+  <si>
+    <t>HPA-1.6X8-SUS</t>
   </si>
 </sst>
 </file>
@@ -492,14 +498,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -819,7 +825,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -871,7 +877,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -904,7 +910,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -932,7 +938,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -963,7 +969,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -994,7 +1000,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -1024,7 +1030,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1052,7 +1058,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1079,7 +1085,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>64</v>
       </c>
@@ -1104,7 +1110,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="8"/>
       <c r="D10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1129,7 +1135,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C11" t="s">
@@ -1159,7 +1165,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="8"/>
       <c r="C12" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1193,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1214,7 +1220,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="8"/>
       <c r="D14" s="1" t="s">
         <v>82</v>
       </c>
@@ -1239,7 +1245,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="8"/>
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1297,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
@@ -1313,20 +1319,20 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>35</v>
       </c>
@@ -1346,18 +1352,18 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1387,7 +1393,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="10"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
         <v>39</v>
@@ -1413,7 +1419,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="2"/>
@@ -1441,7 +1447,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
         <v>43</v>
@@ -1467,7 +1473,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="10"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
         <v>44</v>
@@ -1493,7 +1499,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="10"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
         <v>45</v>
@@ -1519,7 +1525,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="2"/>
@@ -1547,7 +1553,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="10"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>47</v>
@@ -1573,7 +1579,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="10"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>48</v>
@@ -1599,7 +1605,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3" t="s">
         <v>49</v>
@@ -1625,7 +1631,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1655,7 +1661,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="8"/>
       <c r="D30" s="1" t="s">
         <v>91</v>
       </c>
@@ -1678,15 +1684,21 @@
       <c r="D31" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="E31" t="s">
+        <v>100</v>
+      </c>
       <c r="G31" s="7">
         <v>4</v>
       </c>
       <c r="H31" s="7">
-        <v>7</v>
+        <v>5.4</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>21.6</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -1764,22 +1776,22 @@
       </c>
       <c r="I35">
         <f>SUM(I2:I34)</f>
-        <v>185998.25</v>
+        <v>185991.85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="J17:O18"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1794,8 +1806,9 @@
     <hyperlink ref="J16" r:id="rId9" display="https://item.taobao.com/item.htm?id=582286161723&amp;ali_refid=a3_430673_1006:1184860040:N:F%2B7KYUD%2FD3SIN%2BPcInLCJxBrJqj1zio1:329b5c05201caaaba83558623b89cd20&amp;ali_trackid=1_329b5c05201caaaba83558623b89cd20&amp;spm=a2e0b.20350158.31919782.12" xr:uid="{C1BDAF56-2FD3-48FD-9496-E956186D7263}"/>
     <hyperlink ref="J17" r:id="rId10" location="detail" display="https://item.taobao.com/item.htm?spm=a230r.1.14.36.3ce538a7w06UFg&amp;id=652351358299&amp;ns=1&amp;abbucket=8 - detail" xr:uid="{3B27BA99-FB1E-4D78-B787-9FBB5483C4FF}"/>
     <hyperlink ref="J29" r:id="rId11" display="https://www.misumi.com.cn/vona2/detail/221000596791/?pageName=PageCategory" xr:uid="{BFBA29D5-BEDA-49B9-B284-595BCFE20C5F}"/>
+    <hyperlink ref="J31" r:id="rId12" display="https://www.misumi.com.cn/vona2/detail/221000596791/?pageName=PageCategory&amp;CategorySpec=00000235880::a%0900000235872::mig00000001142355%0900000235875::mig00000001130878%0900000235871::b" xr:uid="{0CA1B60A-A186-42A6-B74D-D3A40B34E3C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
send to factory 20210930
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\yj\microscope_design\LaserBox\micolaser_1400_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8249880B-FBA2-49F2-9478-C6956FBA50DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC51BA8-1D0F-45CA-890D-48A6677F2F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DFEBBC-1571-4440-9336-F0CA4138F7AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DFEBBC-1571-4440-9336-F0CA4138F7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -410,6 +410,10 @@
   </si>
   <si>
     <t>HPA-1.6X8-SUS</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a230r.1.14.1.5ab23954NWDenb&amp;id=530385435625&amp;ns=1&amp;abbucket=15#detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -498,14 +502,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -825,7 +829,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -877,7 +881,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -910,7 +914,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -938,7 +942,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -969,7 +973,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +1004,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -1030,7 +1034,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1058,7 +1062,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1085,7 +1089,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="D9" s="1" t="s">
         <v>64</v>
       </c>
@@ -1110,7 +1114,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="9"/>
       <c r="D10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1135,7 +1139,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C11" t="s">
@@ -1165,7 +1169,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="C12" t="s">
         <v>29</v>
       </c>
@@ -1193,7 +1197,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1220,7 +1224,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="9"/>
       <c r="D14" s="1" t="s">
         <v>82</v>
       </c>
@@ -1245,7 +1249,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1297,7 +1301,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
@@ -1319,20 +1323,20 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="9"/>
       <c r="C18" t="s">
         <v>35</v>
       </c>
@@ -1352,18 +1356,18 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1393,7 +1397,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
         <v>39</v>
@@ -1419,7 +1423,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="2"/>
@@ -1447,7 +1451,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
         <v>43</v>
@@ -1473,7 +1477,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
         <v>44</v>
@@ -1499,7 +1503,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
         <v>45</v>
@@ -1525,7 +1529,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="2"/>
@@ -1553,7 +1557,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>47</v>
@@ -1579,7 +1583,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="9"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>48</v>
@@ -1605,7 +1609,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3" t="s">
         <v>49</v>
@@ -1631,7 +1635,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1661,7 +1665,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="9"/>
       <c r="D30" s="1" t="s">
         <v>91</v>
       </c>
@@ -1669,11 +1673,14 @@
         <v>8</v>
       </c>
       <c r="H30" s="7">
-        <v>7</v>
+        <v>0.1</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>0.8</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -1776,22 +1783,22 @@
       </c>
       <c r="I35">
         <f>SUM(I2:I34)</f>
-        <v>185991.85</v>
+        <v>185936.65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="J17:O18"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1807,8 +1814,9 @@
     <hyperlink ref="J17" r:id="rId10" location="detail" display="https://item.taobao.com/item.htm?spm=a230r.1.14.36.3ce538a7w06UFg&amp;id=652351358299&amp;ns=1&amp;abbucket=8 - detail" xr:uid="{3B27BA99-FB1E-4D78-B787-9FBB5483C4FF}"/>
     <hyperlink ref="J29" r:id="rId11" display="https://www.misumi.com.cn/vona2/detail/221000596791/?pageName=PageCategory" xr:uid="{BFBA29D5-BEDA-49B9-B284-595BCFE20C5F}"/>
     <hyperlink ref="J31" r:id="rId12" display="https://www.misumi.com.cn/vona2/detail/221000596791/?pageName=PageCategory&amp;CategorySpec=00000235880::a%0900000235872::mig00000001142355%0900000235875::mig00000001130878%0900000235871::b" xr:uid="{0CA1B60A-A186-42A6-B74D-D3A40B34E3C2}"/>
+    <hyperlink ref="J30" r:id="rId13" location="detail" xr:uid="{84364B0D-9649-4613-8397-84F793EE9B69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>